<commit_message>
Update TestCase template Excel files and remove temporary file
</commit_message>
<xml_diff>
--- a/04.Exercises/Session-04/TestCase-template-1 (Basic).xlsx
+++ b/04.Exercises/Session-04/TestCase-template-1 (Basic).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/GitHub/Aptech/tester-tutorials/04.Exercises/Session-04/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D34338D-7731-6140-A095-E69143B7F678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EE6E5C-B04A-3843-A855-C14B9EFEBE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27200" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case (Basic)" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Dependencies:</t>
   </si>
@@ -227,9 +227,6 @@
   </si>
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>Description</t>
   </si>
   <si>
     <t>Name / Title</t>
@@ -296,6 +293,36 @@
   </si>
   <si>
     <t>Summary Report, Error (0%)</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-01</t>
+  </si>
+  <si>
+    <t>Đăng nhập thành công với username / password hợp lệ</t>
+  </si>
+  <si>
+    <t>Description (Optional)</t>
+  </si>
+  <si>
+    <t>- Truy cập địa chỉ: https://shop.vn/login
+- nhập dữ liệu vào 2 ô nhập liệu username và password
+- Click chuột vào nút Đăng nhập</t>
+  </si>
+  <si>
+    <t>- username: admin
+- password: Abc@123456</t>
+  </si>
+  <si>
+    <t>Hệ thống thông báo đăng nhập thành công và chuyển sang trang chủ</t>
+  </si>
+  <si>
+    <t>Hệ thống có thông báo đăng nhập thành công, nhưng lại chuyển sang trang update profile.</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>Video quay lại có tên: TC-LOGIN-01.mp4</t>
   </si>
 </sst>
 </file>
@@ -528,7 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -641,6 +668,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -660,9 +690,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -700,7 +730,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -806,7 +836,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -948,7 +978,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -958,14 +988,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J347"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="3" ySplit="10" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="1" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <pane xSplit="3" ySplit="10" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.5" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="4" customWidth="1"/>
@@ -976,11 +1006,11 @@
     <col min="7" max="7" width="14" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" style="4" customWidth="1"/>
     <col min="9" max="9" width="4" style="4" customWidth="1"/>
-    <col min="10" max="10" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="11.5" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="37"/>
       <c r="B1" s="37" t="s">
         <v>16</v>
@@ -1002,14 +1032,14 @@
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="38"/>
       <c r="B2" s="38"/>
       <c r="C2" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>4</v>
@@ -1022,7 +1052,7 @@
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="9" t="s">
@@ -1040,7 +1070,7 @@
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="17"/>
       <c r="B4" s="17"/>
       <c r="C4" s="18"/>
@@ -1054,7 +1084,7 @@
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="20"/>
       <c r="B5" s="20"/>
       <c r="C5" s="21"/>
@@ -1112,7 +1142,7 @@
       <c r="I8" s="40"/>
       <c r="J8" s="41"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="26"/>
       <c r="B9" s="26"/>
       <c r="C9" s="21"/>
@@ -1132,10 +1162,10 @@
         <v>26</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E10" s="27" t="s">
         <v>8</v>
@@ -1161,20 +1191,20 @@
         <v>1</v>
       </c>
       <c r="B11" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="D11" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="E11" s="30" t="s">
         <v>32</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>33</v>
       </c>
       <c r="F11" s="30"/>
       <c r="G11" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11" s="31"/>
       <c r="I11" s="32"/>
@@ -1186,19 +1216,19 @@
       </c>
       <c r="B12" s="29"/>
       <c r="C12" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="E12" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="F12" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="G12" s="30" t="s">
         <v>38</v>
-      </c>
-      <c r="G12" s="30" t="s">
-        <v>39</v>
       </c>
       <c r="H12" s="33"/>
       <c r="I12" s="34"/>
@@ -1210,43 +1240,43 @@
       </c>
       <c r="B13" s="29"/>
       <c r="C13" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="30" t="s">
         <v>41</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="30" t="s">
-        <v>42</v>
       </c>
       <c r="H13" s="33"/>
       <c r="I13" s="34"/>
       <c r="J13" s="33"/>
     </row>
-    <row r="14" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" s="28"/>
       <c r="B14" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="35" t="s">
         <v>44</v>
-      </c>
-      <c r="C14" s="35" t="s">
-        <v>45</v>
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
       <c r="F14" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="28" t="s">
         <v>46</v>
-      </c>
-      <c r="G14" s="28" t="s">
-        <v>47</v>
       </c>
       <c r="H14" s="33"/>
       <c r="I14" s="34"/>
       <c r="J14" s="33"/>
     </row>
-    <row r="15" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A15" s="28"/>
       <c r="B15" s="28"/>
       <c r="C15" s="35"/>
@@ -1258,7 +1288,7 @@
       <c r="I15" s="34"/>
       <c r="J15" s="33"/>
     </row>
-    <row r="16" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" s="28"/>
       <c r="B16" s="28"/>
       <c r="C16" s="35"/>
@@ -1270,19 +1300,37 @@
       <c r="I16" s="34"/>
       <c r="J16" s="33"/>
     </row>
-    <row r="17" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="35"/>
+    <row r="17" spans="1:10" s="8" customFormat="1" ht="204" x14ac:dyDescent="0.15">
+      <c r="A17" s="28">
+        <v>4</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>48</v>
+      </c>
       <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="33"/>
-    </row>
-    <row r="18" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="E17" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="J17" s="33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" s="28"/>
       <c r="B18" s="28"/>
       <c r="C18" s="35"/>
@@ -1294,7 +1342,7 @@
       <c r="I18" s="34"/>
       <c r="J18" s="33"/>
     </row>
-    <row r="19" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" s="28"/>
       <c r="B19" s="28"/>
       <c r="C19" s="35"/>

</xml_diff>

<commit_message>
chore: Update TestCase template with latest project data
</commit_message>
<xml_diff>
--- a/04.Exercises/Session-04/TestCase-template-1 (Basic).xlsx
+++ b/04.Exercises/Session-04/TestCase-template-1 (Basic).xlsx
@@ -1,22 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/GitHub/Aptech/tester-tutorials/04.Exercises/Session-04/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EE6E5C-B04A-3843-A855-C14B9EFEBE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D4EF00-EC4E-C445-A990-DB3B5AF4209D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case (Basic)" sheetId="1" r:id="rId1"/>
-    <sheet name="METADATA" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="METADATA" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="101716"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -65,7 +79,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -74,12 +88,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Kết quả thực tế khi thực thi với TEST DATA</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kết quả thực tế khi thực thi với TEST DATA</t>
         </r>
       </text>
     </comment>
@@ -146,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>Dependencies:</t>
   </si>
@@ -283,18 +306,6 @@
 2. </t>
   </si>
   <si>
-    <t>TC-P-1000R-1S</t>
-  </si>
-  <si>
-    <t>Thực hiện load test cho API: ./register</t>
-  </si>
-  <si>
-    <t>TC-123 (JMETER)</t>
-  </si>
-  <si>
-    <t>Summary Report, Error (0%)</t>
-  </si>
-  <si>
     <t>TC-LOGIN-01</t>
   </si>
   <si>
@@ -323,6 +334,41 @@
   </si>
   <si>
     <t>Video quay lại có tên: TC-LOGIN-01.mp4</t>
+  </si>
+  <si>
+    <t>TC-ORDER-FULLNAME-01</t>
+  </si>
+  <si>
+    <t>Họ và tên bắt buộc phải nhập</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Nhập họ và tên vào ô Họ và tên trên form
+2. 
+3. </t>
+  </si>
+  <si>
+    <t>Không có bất kỳ thông báo lỗi nào xuất liên quan đến Họ và tên</t>
+  </si>
+  <si>
+    <t>Họ và tên = Nguyễn Tuân</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>TC-ORDER-FULLNAME-02</t>
+  </si>
+  <si>
+    <t>Họ và tên nhập 100 ký tự</t>
+  </si>
+  <si>
+    <t>Họ và tên nhập 99 ký tự</t>
+  </si>
+  <si>
+    <t>TC-ORDER-FULLNAME-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyen Van Tuan Nguyen Van Tuan </t>
   </si>
 </sst>
 </file>
@@ -555,7 +601,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -653,6 +699,9 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -668,8 +717,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -989,10 +1038,10 @@
   <dimension ref="A1:J347"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="3" ySplit="10" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="10" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1011,8 +1060,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="37"/>
-      <c r="B1" s="37" t="s">
+      <c r="A1" s="38"/>
+      <c r="B1" s="38" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="9" t="s">
@@ -1033,8 +1082,8 @@
       <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="9" t="s">
         <v>13</v>
       </c>
@@ -1101,46 +1150,46 @@
       <c r="B6" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="42"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25"/>
       <c r="B7" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="41"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="42"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25"/>
       <c r="B8" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="42"/>
     </row>
     <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="26"/>
@@ -1165,7 +1214,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E10" s="27" t="s">
         <v>8</v>
@@ -1256,48 +1305,76 @@
       <c r="I13" s="34"/>
       <c r="J13" s="33"/>
     </row>
-    <row r="14" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A14" s="28"/>
       <c r="B14" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="35" t="s">
-        <v>44</v>
+        <v>52</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>53</v>
       </c>
       <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
+      <c r="E14" s="30" t="s">
+        <v>54</v>
+      </c>
       <c r="F14" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="28" t="s">
-        <v>46</v>
+        <v>56</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>55</v>
       </c>
       <c r="H14" s="33"/>
-      <c r="I14" s="34"/>
+      <c r="I14" s="34" t="s">
+        <v>57</v>
+      </c>
       <c r="J14" s="33"/>
     </row>
-    <row r="15" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="35"/>
+      <c r="B15" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>59</v>
+      </c>
       <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
+      <c r="E15" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>55</v>
+      </c>
       <c r="H15" s="33"/>
-      <c r="I15" s="34"/>
+      <c r="I15" s="34" t="s">
+        <v>57</v>
+      </c>
       <c r="J15" s="33"/>
     </row>
-    <row r="16" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="35"/>
+      <c r="B16" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>60</v>
+      </c>
       <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
+      <c r="E16" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>55</v>
+      </c>
       <c r="H16" s="33"/>
-      <c r="I16" s="34"/>
+      <c r="I16" s="34" t="s">
+        <v>57</v>
+      </c>
       <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10" s="8" customFormat="1" ht="204" x14ac:dyDescent="0.15">
@@ -1305,29 +1382,29 @@
         <v>4</v>
       </c>
       <c r="B17" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="G17" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="42" t="s">
+      <c r="H17" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="J17" s="33" t="s">
         <v>51</v>
-      </c>
-      <c r="G17" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="H17" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="J17" s="33" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
@@ -5313,6 +5390,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C3C3D3-3A15-B64B-B118-0629A7CC7B15}">
+  <dimension ref="F20:G20"/>
+  <sheetViews>
+    <sheetView topLeftCell="E11" zoomScale="374" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.15">
+      <c r="F20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20">
+        <f>LEN(F20)</f>
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>

</xml_diff>